<commit_message>
updated UC-Spec.docx and Requirements-Table.xlsx documents
</commit_message>
<xml_diff>
--- a/Docs/Requirements-Table.xlsx
+++ b/Docs/Requirements-Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feodor\Desktop\project\segroup9\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Terkel\OneDrive\Study\SE\git\segroup9\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB73848-3EF0-4227-B996-F3B39B5D2A21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C6BD87-F8D1-4DA2-B621-56A209CDF887}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="דרישות" sheetId="1" r:id="rId1"/>
@@ -22,8 +22,8 @@
     <definedName name="HML">'סוגי דרישות'!#REF!</definedName>
     <definedName name="NFR">'סוגי דרישות'!$B$10:$B$14</definedName>
     <definedName name="OLE_LINK1" localSheetId="0">דרישות!$B$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">דרישות!$A$3:$E$13</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">דרישות!$4:$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">דרישות!$A$3:$E$13</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="117">
   <si>
     <t>זיהוי</t>
   </si>
@@ -285,13 +285,7 @@
     </r>
   </si>
   <si>
-    <t>בהגדרה עצית ניתן לבחור סוג פריט</t>
-  </si>
-  <si>
     <t>בהגדרה עצית ניתן לבחור צבע שולט</t>
-  </si>
-  <si>
-    <t>בהגדרה עצית ניתן לבחור טווח מחירים</t>
   </si>
   <si>
     <r>
@@ -896,6 +890,24 @@
   </si>
   <si>
     <t>סיפור לקוח</t>
+  </si>
+  <si>
+    <t>יכולת חיפוש בקטלוג</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>יכולת טיפול בתלונה</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>בהגדרה עצית יש לבחור סוג פריט</t>
+  </si>
+  <si>
+    <t>בהגדרה עצית יש לבחור טווח מחירים</t>
   </si>
 </sst>
 </file>
@@ -1354,7 +1366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -1548,9 +1560,6 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="2"/>
     </xf>
@@ -1600,6 +1609,15 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1636,18 +1654,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1663,9 +1681,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1703,7 +1721,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1809,7 +1827,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1989,8 +2007,8 @@
   <dimension ref="A1:H80"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2012,10 +2030,10 @@
       <c r="B1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="91"/>
+      <c r="D1" s="93"/>
       <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1">
@@ -2025,8 +2043,8 @@
       <c r="B2" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="91"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="93"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="1"/>
@@ -2044,42 +2062,42 @@
       <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="89"/>
-      <c r="F4" s="87" t="s">
+      <c r="E4" s="91"/>
+      <c r="F4" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="88"/>
-      <c r="H4" s="89"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="91"/>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A5" s="96"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="98"/>
+      <c r="A5" s="98"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="100"/>
       <c r="D5" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="80" t="s">
+      <c r="F5" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="80" t="s">
+      <c r="G5" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="80" t="s">
+      <c r="H5" s="79" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2088,18 +2106,18 @@
         <v>1</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D6" s="52"/>
       <c r="E6" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="81"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="74"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="73"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="53">
@@ -2109,7 +2127,7 @@
         <v>46</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>6</v>
@@ -2119,7 +2137,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="24"/>
-      <c r="H7" s="75"/>
+      <c r="H7" s="74"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="53">
@@ -2129,7 +2147,7 @@
         <v>47</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="20" t="s">
@@ -2137,7 +2155,7 @@
       </c>
       <c r="F8" s="43"/>
       <c r="G8" s="24"/>
-      <c r="H8" s="75"/>
+      <c r="H8" s="74"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="53">
@@ -2147,7 +2165,7 @@
         <v>38</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="20" t="s">
@@ -2157,7 +2175,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="24"/>
-      <c r="H9" s="75"/>
+      <c r="H9" s="74"/>
     </row>
     <row r="10" spans="1:8" ht="12.6" customHeight="1">
       <c r="A10" s="53">
@@ -2167,7 +2185,7 @@
         <v>48</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>6</v>
@@ -2177,7 +2195,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="24"/>
-      <c r="H10" s="75"/>
+      <c r="H10" s="74"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="53">
@@ -2187,7 +2205,7 @@
         <v>49</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>6</v>
@@ -2197,17 +2215,17 @@
         <v>4</v>
       </c>
       <c r="G11" s="24"/>
-      <c r="H11" s="75"/>
+      <c r="H11" s="74"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="53">
         <v>7</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>6</v>
@@ -2217,17 +2235,17 @@
         <v>4</v>
       </c>
       <c r="G12" s="24"/>
-      <c r="H12" s="75"/>
+      <c r="H12" s="74"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="53">
         <v>8</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>6</v>
@@ -2237,17 +2255,17 @@
         <v>4</v>
       </c>
       <c r="G13" s="24"/>
-      <c r="H13" s="75"/>
+      <c r="H13" s="74"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="53">
         <v>9</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>6</v>
@@ -2257,17 +2275,17 @@
         <v>4</v>
       </c>
       <c r="G14" s="24"/>
-      <c r="H14" s="75"/>
+      <c r="H14" s="74"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="53">
         <v>10</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>6</v>
@@ -2277,17 +2295,17 @@
         <v>7</v>
       </c>
       <c r="G15" s="24"/>
-      <c r="H15" s="75"/>
+      <c r="H15" s="74"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="53">
         <v>11</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>6</v>
@@ -2297,17 +2315,17 @@
         <v>7</v>
       </c>
       <c r="G16" s="24"/>
-      <c r="H16" s="75"/>
+      <c r="H16" s="74"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="53">
         <v>12</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="19" t="s">
@@ -2317,17 +2335,17 @@
         <v>7</v>
       </c>
       <c r="G17" s="24"/>
-      <c r="H17" s="75"/>
+      <c r="H17" s="74"/>
     </row>
     <row r="18" spans="1:8" s="33" customFormat="1">
       <c r="A18" s="53">
         <v>13</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>6</v>
@@ -2337,17 +2355,17 @@
         <v>7</v>
       </c>
       <c r="G18" s="32"/>
-      <c r="H18" s="82"/>
+      <c r="H18" s="81"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="53">
         <v>14</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D19" s="19" t="s">
         <v>6</v>
@@ -2357,17 +2375,17 @@
         <v>7</v>
       </c>
       <c r="G19" s="27"/>
-      <c r="H19" s="75"/>
+      <c r="H19" s="74"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="53">
         <v>15</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>6</v>
@@ -2377,17 +2395,17 @@
         <v>7</v>
       </c>
       <c r="G20" s="27"/>
-      <c r="H20" s="75"/>
+      <c r="H20" s="74"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="53">
         <v>16</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>6</v>
@@ -2397,17 +2415,17 @@
         <v>7</v>
       </c>
       <c r="G21" s="27"/>
-      <c r="H21" s="75"/>
+      <c r="H21" s="74"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="53">
         <v>17</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="19" t="s">
@@ -2415,17 +2433,17 @@
       </c>
       <c r="F22" s="43"/>
       <c r="G22" s="27"/>
-      <c r="H22" s="75"/>
+      <c r="H22" s="74"/>
     </row>
     <row r="23" spans="1:8" ht="25.5">
       <c r="A23" s="53">
         <v>18</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="19" t="s">
@@ -2433,17 +2451,17 @@
       </c>
       <c r="F23" s="44"/>
       <c r="G23" s="27"/>
-      <c r="H23" s="77"/>
+      <c r="H23" s="76"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="53">
         <v>19</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>6</v>
@@ -2455,17 +2473,17 @@
         <v>7</v>
       </c>
       <c r="G24" s="27"/>
-      <c r="H24" s="75"/>
+      <c r="H24" s="74"/>
     </row>
     <row r="25" spans="1:8" s="33" customFormat="1" ht="25.5">
       <c r="A25" s="55">
         <v>20</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20" t="s">
@@ -2473,17 +2491,17 @@
       </c>
       <c r="F25" s="42"/>
       <c r="G25" s="40"/>
-      <c r="H25" s="82"/>
+      <c r="H25" s="81"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="53">
         <v>21</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="19" t="s">
@@ -2491,17 +2509,17 @@
       </c>
       <c r="F26" s="43"/>
       <c r="G26" s="24"/>
-      <c r="H26" s="75"/>
+      <c r="H26" s="74"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="53">
         <v>22</v>
       </c>
       <c r="B27" s="56" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>6</v>
@@ -2509,7 +2527,7 @@
       <c r="E27" s="19"/>
       <c r="F27" s="43"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="75"/>
+      <c r="H27" s="74"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="53">
@@ -2519,7 +2537,7 @@
         <v>39</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>6</v>
@@ -2529,17 +2547,17 @@
         <v>7</v>
       </c>
       <c r="G28" s="24"/>
-      <c r="H28" s="75"/>
+      <c r="H28" s="74"/>
     </row>
     <row r="29" spans="1:8" ht="13.5" thickBot="1">
       <c r="A29" s="57">
         <v>24</v>
       </c>
       <c r="B29" s="58" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C29" s="47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D29" s="63" t="s">
         <v>10</v>
@@ -2549,37 +2567,37 @@
         <v>7</v>
       </c>
       <c r="G29" s="62"/>
-      <c r="H29" s="79"/>
+      <c r="H29" s="78"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="53">
         <v>25</v>
       </c>
-      <c r="B30" s="71" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="100" t="s">
-        <v>112</v>
+      <c r="B30" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="87" t="s">
+        <v>110</v>
       </c>
       <c r="D30" s="52" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="52"/>
-      <c r="F30" s="72">
+      <c r="F30" s="71">
         <v>3</v>
       </c>
-      <c r="G30" s="73"/>
-      <c r="H30" s="74"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="73"/>
     </row>
     <row r="31" spans="1:8" ht="13.5" thickBot="1">
       <c r="A31" s="57">
         <v>26</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>10</v>
@@ -2589,37 +2607,37 @@
         <v>3</v>
       </c>
       <c r="G31" s="27"/>
-      <c r="H31" s="75"/>
+      <c r="H31" s="74"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="53">
         <v>27</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E32" s="19"/>
       <c r="F32" s="24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G32" s="24"/>
-      <c r="H32" s="75"/>
+      <c r="H32" s="74"/>
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1">
       <c r="A33" s="57">
         <v>28</v>
       </c>
-      <c r="B33" s="76" t="s">
-        <v>71</v>
+      <c r="B33" s="75" t="s">
+        <v>69</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>10</v>
@@ -2629,17 +2647,17 @@
         <v>3</v>
       </c>
       <c r="G33" s="24"/>
-      <c r="H33" s="75"/>
+      <c r="H33" s="74"/>
     </row>
     <row r="34" spans="1:8" ht="15">
       <c r="A34" s="53">
         <v>29</v>
       </c>
-      <c r="B34" s="76" t="s">
-        <v>72</v>
+      <c r="B34" s="75" t="s">
+        <v>70</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>6</v>
@@ -2649,17 +2667,17 @@
         <v>3.7</v>
       </c>
       <c r="G34" s="24"/>
-      <c r="H34" s="75"/>
+      <c r="H34" s="74"/>
     </row>
     <row r="35" spans="1:8" ht="13.5" thickBot="1">
       <c r="A35" s="57">
         <v>30</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>10</v>
@@ -2667,17 +2685,17 @@
       <c r="E35" s="19"/>
       <c r="F35" s="24"/>
       <c r="G35" s="24"/>
-      <c r="H35" s="75"/>
+      <c r="H35" s="74"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="53">
         <v>31</v>
       </c>
       <c r="B36" s="65" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>6</v>
@@ -2687,17 +2705,17 @@
         <v>9</v>
       </c>
       <c r="G36" s="24"/>
-      <c r="H36" s="77"/>
+      <c r="H36" s="76"/>
     </row>
     <row r="37" spans="1:8" ht="13.5" thickBot="1">
       <c r="A37" s="57">
         <v>32</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D37" s="19"/>
       <c r="E37" s="19" t="s">
@@ -2707,17 +2725,17 @@
         <v>9</v>
       </c>
       <c r="G37" s="24"/>
-      <c r="H37" s="75"/>
+      <c r="H37" s="74"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="53">
         <v>33</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19" t="s">
@@ -2727,17 +2745,17 @@
         <v>9</v>
       </c>
       <c r="G38" s="24"/>
-      <c r="H38" s="75"/>
+      <c r="H38" s="74"/>
     </row>
     <row r="39" spans="1:8" ht="13.5" thickBot="1">
       <c r="A39" s="57">
         <v>34</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="19" t="s">
@@ -2747,17 +2765,17 @@
         <v>9</v>
       </c>
       <c r="G39" s="27"/>
-      <c r="H39" s="75"/>
+      <c r="H39" s="74"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="53">
         <v>35</v>
       </c>
       <c r="B40" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" s="99" t="s">
-        <v>57</v>
+        <v>76</v>
+      </c>
+      <c r="C40" s="86" t="s">
+        <v>55</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>6</v>
@@ -2767,17 +2785,17 @@
       </c>
       <c r="F40" s="24"/>
       <c r="G40" s="24"/>
-      <c r="H40" s="75"/>
+      <c r="H40" s="74"/>
     </row>
     <row r="41" spans="1:8" ht="13.5" thickBot="1">
       <c r="A41" s="57">
         <v>36</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>6</v>
@@ -2787,17 +2805,17 @@
         <v>9</v>
       </c>
       <c r="G41" s="24"/>
-      <c r="H41" s="75"/>
+      <c r="H41" s="74"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="53">
         <v>37</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D42" s="19" t="s">
         <v>6</v>
@@ -2807,17 +2825,17 @@
         <v>10</v>
       </c>
       <c r="G42" s="24"/>
-      <c r="H42" s="75"/>
+      <c r="H42" s="74"/>
     </row>
     <row r="43" spans="1:8" ht="13.5" thickBot="1">
       <c r="A43" s="57">
         <v>38</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="19" t="s">
@@ -2827,17 +2845,17 @@
         <v>11</v>
       </c>
       <c r="G43" s="24"/>
-      <c r="H43" s="75"/>
+      <c r="H43" s="74"/>
     </row>
     <row r="44" spans="1:8" ht="13.5" thickBot="1">
       <c r="A44" s="53">
         <v>39</v>
       </c>
-      <c r="B44" s="78" t="s">
-        <v>82</v>
+      <c r="B44" s="77" t="s">
+        <v>80</v>
       </c>
       <c r="C44" s="47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D44" s="48"/>
       <c r="E44" s="48" t="s">
@@ -2845,35 +2863,35 @@
       </c>
       <c r="F44" s="64"/>
       <c r="G44" s="64"/>
-      <c r="H44" s="79"/>
+      <c r="H44" s="78"/>
     </row>
     <row r="45" spans="1:8" ht="13.5" thickBot="1">
       <c r="A45" s="57">
         <v>40</v>
       </c>
-      <c r="B45" s="83" t="s">
+      <c r="B45" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="100" t="s">
-        <v>112</v>
+      <c r="C45" s="87" t="s">
+        <v>110</v>
       </c>
       <c r="D45" s="52" t="s">
         <v>6</v>
       </c>
       <c r="E45" s="52"/>
-      <c r="F45" s="73"/>
-      <c r="G45" s="73"/>
-      <c r="H45" s="74"/>
+      <c r="F45" s="72"/>
+      <c r="G45" s="72"/>
+      <c r="H45" s="73"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="53">
         <v>41</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="19" t="s">
@@ -2881,7 +2899,7 @@
       </c>
       <c r="F46" s="24"/>
       <c r="G46" s="24"/>
-      <c r="H46" s="75"/>
+      <c r="H46" s="74"/>
     </row>
     <row r="47" spans="1:8" ht="13.5" thickBot="1">
       <c r="A47" s="57">
@@ -2891,7 +2909,7 @@
         <v>40</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D47" s="19" t="s">
         <v>6</v>
@@ -2901,17 +2919,17 @@
         <v>12</v>
       </c>
       <c r="G47" s="24"/>
-      <c r="H47" s="75"/>
+      <c r="H47" s="74"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="53">
         <v>43</v>
       </c>
       <c r="B48" s="65" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" s="99" t="s">
-        <v>57</v>
+        <v>82</v>
+      </c>
+      <c r="C48" s="86" t="s">
+        <v>55</v>
       </c>
       <c r="D48" s="19" t="s">
         <v>10</v>
@@ -2919,17 +2937,17 @@
       <c r="E48" s="19"/>
       <c r="F48" s="24"/>
       <c r="G48" s="24"/>
-      <c r="H48" s="75"/>
+      <c r="H48" s="74"/>
     </row>
     <row r="49" spans="1:8" ht="13.5" thickBot="1">
       <c r="A49" s="57">
         <v>44</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="19" t="s">
@@ -2939,17 +2957,17 @@
         <v>7</v>
       </c>
       <c r="G49" s="24"/>
-      <c r="H49" s="75"/>
+      <c r="H49" s="74"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="53">
         <v>45</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D50" s="19"/>
       <c r="E50" s="19" t="s">
@@ -2959,17 +2977,17 @@
         <v>7</v>
       </c>
       <c r="G50" s="24"/>
-      <c r="H50" s="75"/>
+      <c r="H50" s="74"/>
     </row>
     <row r="51" spans="1:8" ht="13.5" thickBot="1">
       <c r="A51" s="57">
         <v>46</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D51" s="19"/>
       <c r="E51" s="19" t="s">
@@ -2979,37 +2997,37 @@
         <v>11.1</v>
       </c>
       <c r="G51" s="24"/>
-      <c r="H51" s="75"/>
+      <c r="H51" s="74"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="53">
         <v>47</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D52" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E52" s="84"/>
+      <c r="E52" s="83"/>
       <c r="F52" s="24">
         <v>12</v>
       </c>
       <c r="G52" s="24"/>
-      <c r="H52" s="75"/>
+      <c r="H52" s="74"/>
     </row>
     <row r="53" spans="1:8" ht="13.5" thickBot="1">
       <c r="A53" s="57">
         <v>48</v>
       </c>
       <c r="B53" s="58" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C53" s="47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D53" s="48" t="s">
         <v>6</v>
@@ -3019,37 +3037,37 @@
         <v>12</v>
       </c>
       <c r="G53" s="64"/>
-      <c r="H53" s="79"/>
+      <c r="H53" s="78"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="53">
         <v>49</v>
       </c>
-      <c r="B54" s="85" t="s">
-        <v>90</v>
-      </c>
-      <c r="C54" s="101" t="s">
-        <v>57</v>
+      <c r="B54" s="84" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="88" t="s">
+        <v>55</v>
       </c>
       <c r="D54" s="52" t="s">
         <v>6</v>
       </c>
       <c r="E54" s="52"/>
-      <c r="F54" s="73">
+      <c r="F54" s="72">
         <v>1</v>
       </c>
-      <c r="G54" s="73"/>
-      <c r="H54" s="74"/>
+      <c r="G54" s="72"/>
+      <c r="H54" s="73"/>
     </row>
     <row r="55" spans="1:8" ht="13.5" thickBot="1">
       <c r="A55" s="57">
         <v>50</v>
       </c>
       <c r="B55" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="C55" s="99" t="s">
-        <v>57</v>
+        <v>90</v>
+      </c>
+      <c r="C55" s="86" t="s">
+        <v>55</v>
       </c>
       <c r="D55" s="19" t="s">
         <v>10</v>
@@ -3059,17 +3077,17 @@
         <v>1</v>
       </c>
       <c r="G55" s="24"/>
-      <c r="H55" s="75"/>
+      <c r="H55" s="74"/>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="53">
         <v>51</v>
       </c>
       <c r="B56" s="34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D56" s="19"/>
       <c r="E56" s="19" t="s">
@@ -3077,17 +3095,17 @@
       </c>
       <c r="F56" s="24"/>
       <c r="G56" s="24"/>
-      <c r="H56" s="75"/>
+      <c r="H56" s="74"/>
     </row>
     <row r="57" spans="1:8" ht="13.5" thickBot="1">
       <c r="A57" s="57">
         <v>52</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D57" s="19"/>
       <c r="E57" s="19" t="s">
@@ -3097,17 +3115,17 @@
         <v>2.7</v>
       </c>
       <c r="G57" s="24"/>
-      <c r="H57" s="75"/>
+      <c r="H57" s="74"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="53">
         <v>53</v>
       </c>
       <c r="B58" s="65" t="s">
-        <v>94</v>
-      </c>
-      <c r="C58" s="99" t="s">
-        <v>57</v>
+        <v>92</v>
+      </c>
+      <c r="C58" s="86" t="s">
+        <v>55</v>
       </c>
       <c r="D58" s="19" t="s">
         <v>6</v>
@@ -3117,17 +3135,17 @@
         <v>8</v>
       </c>
       <c r="G58" s="24"/>
-      <c r="H58" s="75"/>
+      <c r="H58" s="74"/>
     </row>
     <row r="59" spans="1:8" ht="13.5" thickBot="1">
       <c r="A59" s="57">
         <v>54</v>
       </c>
       <c r="B59" s="31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D59" s="19" t="s">
         <v>6</v>
@@ -3137,17 +3155,17 @@
         <v>7</v>
       </c>
       <c r="G59" s="24"/>
-      <c r="H59" s="75"/>
+      <c r="H59" s="74"/>
     </row>
     <row r="60" spans="1:8" ht="25.5">
       <c r="A60" s="53">
         <v>55</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D60" s="19" t="s">
         <v>6</v>
@@ -3157,7 +3175,7 @@
         <v>7</v>
       </c>
       <c r="G60" s="24"/>
-      <c r="H60" s="75"/>
+      <c r="H60" s="74"/>
     </row>
     <row r="61" spans="1:8" ht="26.25" thickBot="1">
       <c r="A61" s="57">
@@ -3167,7 +3185,7 @@
         <v>44</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D61" s="19" t="s">
         <v>6</v>
@@ -3179,17 +3197,17 @@
         <v>8</v>
       </c>
       <c r="G61" s="24"/>
-      <c r="H61" s="75"/>
+      <c r="H61" s="74"/>
     </row>
     <row r="62" spans="1:8" ht="25.5">
       <c r="A62" s="53">
         <v>57</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D62" s="19" t="s">
         <v>6</v>
@@ -3199,17 +3217,17 @@
         <v>2</v>
       </c>
       <c r="G62" s="24"/>
-      <c r="H62" s="75"/>
+      <c r="H62" s="74"/>
     </row>
     <row r="63" spans="1:8" ht="13.5" thickBot="1">
       <c r="A63" s="57">
         <v>58</v>
       </c>
       <c r="B63" s="31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D63" s="19" t="s">
         <v>6</v>
@@ -3219,17 +3237,17 @@
         <v>14</v>
       </c>
       <c r="G63" s="24"/>
-      <c r="H63" s="75"/>
+      <c r="H63" s="74"/>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="53">
         <v>59</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D64" s="19" t="s">
         <v>10</v>
@@ -3237,17 +3255,17 @@
       <c r="E64" s="19"/>
       <c r="F64" s="24"/>
       <c r="G64" s="24"/>
-      <c r="H64" s="75"/>
+      <c r="H64" s="74"/>
     </row>
     <row r="65" spans="1:8" ht="13.5" thickBot="1">
       <c r="A65" s="57">
         <v>60</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D65" s="19" t="s">
         <v>6</v>
@@ -3259,17 +3277,17 @@
         <v>15</v>
       </c>
       <c r="G65" s="24"/>
-      <c r="H65" s="75"/>
+      <c r="H65" s="74"/>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="53">
         <v>61</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D66" s="19"/>
       <c r="E66" s="19" t="s">
@@ -3279,17 +3297,17 @@
         <v>2</v>
       </c>
       <c r="G66" s="24"/>
-      <c r="H66" s="75"/>
+      <c r="H66" s="74"/>
     </row>
     <row r="67" spans="1:8" ht="13.5" thickBot="1">
       <c r="A67" s="57">
         <v>62</v>
       </c>
-      <c r="B67" s="78" t="s">
+      <c r="B67" s="77" t="s">
         <v>45</v>
       </c>
       <c r="C67" s="47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D67" s="48"/>
       <c r="E67" s="48" t="s">
@@ -3299,35 +3317,35 @@
         <v>2</v>
       </c>
       <c r="G67" s="64"/>
-      <c r="H67" s="79"/>
+      <c r="H67" s="78"/>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="53">
         <v>63</v>
       </c>
-      <c r="B68" s="83" t="s">
-        <v>101</v>
-      </c>
-      <c r="C68" s="100" t="s">
-        <v>112</v>
+      <c r="B68" s="82" t="s">
+        <v>99</v>
+      </c>
+      <c r="C68" s="87" t="s">
+        <v>110</v>
       </c>
       <c r="D68" s="52"/>
       <c r="E68" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="F68" s="73"/>
-      <c r="G68" s="73"/>
-      <c r="H68" s="74"/>
+      <c r="F68" s="72"/>
+      <c r="G68" s="72"/>
+      <c r="H68" s="73"/>
     </row>
     <row r="69" spans="1:8" ht="13.5" thickBot="1">
       <c r="A69" s="57">
         <v>64</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D69" s="19"/>
       <c r="E69" s="19" t="s">
@@ -3335,17 +3353,17 @@
       </c>
       <c r="F69" s="24"/>
       <c r="G69" s="24"/>
-      <c r="H69" s="75"/>
+      <c r="H69" s="74"/>
     </row>
     <row r="70" spans="1:8" ht="25.5">
       <c r="A70" s="53">
         <v>65</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D70" s="19"/>
       <c r="E70" s="19" t="s">
@@ -3353,17 +3371,17 @@
       </c>
       <c r="F70" s="24"/>
       <c r="G70" s="24"/>
-      <c r="H70" s="75"/>
+      <c r="H70" s="74"/>
     </row>
     <row r="71" spans="1:8" ht="26.25" thickBot="1">
       <c r="A71" s="57">
         <v>66</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D71" s="19"/>
       <c r="E71" s="19" t="s">
@@ -3371,17 +3389,17 @@
       </c>
       <c r="F71" s="24"/>
       <c r="G71" s="24"/>
-      <c r="H71" s="75"/>
+      <c r="H71" s="74"/>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="53">
         <v>67</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D72" s="19"/>
       <c r="E72" s="19" t="s">
@@ -3389,17 +3407,17 @@
       </c>
       <c r="F72" s="24"/>
       <c r="G72" s="24"/>
-      <c r="H72" s="75"/>
+      <c r="H72" s="74"/>
     </row>
     <row r="73" spans="1:8" ht="13.5" thickBot="1">
       <c r="A73" s="57">
         <v>68</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D73" s="19"/>
       <c r="E73" s="19" t="s">
@@ -3407,17 +3425,17 @@
       </c>
       <c r="F73" s="24"/>
       <c r="G73" s="24"/>
-      <c r="H73" s="75"/>
+      <c r="H73" s="74"/>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="53">
         <v>69</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D74" s="19"/>
       <c r="E74" s="19" t="s">
@@ -3425,17 +3443,17 @@
       </c>
       <c r="F74" s="24"/>
       <c r="G74" s="24"/>
-      <c r="H74" s="75"/>
+      <c r="H74" s="74"/>
     </row>
     <row r="75" spans="1:8" ht="13.5" thickBot="1">
       <c r="A75" s="57">
         <v>70</v>
       </c>
-      <c r="B75" s="86" t="s">
-        <v>108</v>
+      <c r="B75" s="85" t="s">
+        <v>106</v>
       </c>
       <c r="C75" s="47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D75" s="48"/>
       <c r="E75" s="48" t="s">
@@ -3443,25 +3461,45 @@
       </c>
       <c r="F75" s="64"/>
       <c r="G75" s="64"/>
-      <c r="H75" s="79"/>
+      <c r="H75" s="78"/>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="68"/>
-      <c r="B76" s="69"/>
-      <c r="C76" s="70"/>
-      <c r="D76" s="45"/>
+      <c r="A76" s="68" t="s">
+        <v>112</v>
+      </c>
+      <c r="B76" s="101" t="s">
+        <v>111</v>
+      </c>
+      <c r="C76" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="D76" s="45" t="s">
+        <v>6</v>
+      </c>
       <c r="E76" s="45"/>
-      <c r="F76" s="59"/>
+      <c r="F76" s="59">
+        <v>6</v>
+      </c>
       <c r="G76" s="59"/>
       <c r="H76" s="59"/>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" s="66"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="67"/>
-      <c r="D77" s="19"/>
+      <c r="A77" s="102" t="s">
+        <v>114</v>
+      </c>
+      <c r="B77" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="C77" s="103" t="s">
+        <v>55</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>6</v>
+      </c>
       <c r="E77" s="19"/>
-      <c r="F77" s="24"/>
+      <c r="F77" s="24">
+        <v>11</v>
+      </c>
       <c r="G77" s="24"/>
       <c r="H77" s="24"/>
     </row>

</xml_diff>

<commit_message>
updated UC-Spec and Requirements-Table
</commit_message>
<xml_diff>
--- a/Docs/Requirements-Table.xlsx
+++ b/Docs/Requirements-Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Terkel\OneDrive\Study\SE\git\segroup9\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CFE18D-2AFE-43A5-92C8-CB533BE51A6D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE70CE8D-F474-4FD3-B504-0BAEB145B5B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="סוגי דרישות" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">דרישות!$F$1:$F$80</definedName>
     <definedName name="FR">'סוגי דרישות'!$B$5:$B$6</definedName>
     <definedName name="FuncReq">'סוגי דרישות'!$B$5:$B$6</definedName>
     <definedName name="HML">'סוגי דרישות'!#REF!</definedName>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="118">
   <si>
     <t>זיהוי</t>
   </si>
@@ -908,6 +909,9 @@
   </si>
   <si>
     <t>בהגדרה עצית יש לבחור טווח מחירים</t>
+  </si>
+  <si>
+    <t>12, 16</t>
   </si>
 </sst>
 </file>
@@ -1366,7 +1370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -1551,12 +1555,6 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="2"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1618,6 +1616,15 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1654,15 +1661,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2004,11 +2015,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="5" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2030,10 +2041,10 @@
       <c r="B1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="93"/>
+      <c r="D1" s="94"/>
       <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1">
@@ -2043,8 +2054,8 @@
       <c r="B2" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="93"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="94"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="1"/>
@@ -2062,42 +2073,42 @@
       <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="99" t="s">
+      <c r="C4" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="89" t="s">
+      <c r="D4" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="91"/>
-      <c r="F4" s="89" t="s">
+      <c r="E4" s="92"/>
+      <c r="F4" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="92"/>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A5" s="98"/>
-      <c r="B5" s="96"/>
-      <c r="C5" s="100"/>
+      <c r="A5" s="99"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="101"/>
       <c r="D5" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="79" t="s">
+      <c r="F5" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="79" t="s">
+      <c r="G5" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="79" t="s">
+      <c r="H5" s="77" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2115,9 +2126,9 @@
       <c r="E6" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="80"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="73"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="71"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="53">
@@ -2137,7 +2148,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="24"/>
-      <c r="H7" s="74"/>
+      <c r="H7" s="72"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="53">
@@ -2155,7 +2166,7 @@
       </c>
       <c r="F8" s="43"/>
       <c r="G8" s="24"/>
-      <c r="H8" s="74"/>
+      <c r="H8" s="72"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="53">
@@ -2175,7 +2186,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="24"/>
-      <c r="H9" s="74"/>
+      <c r="H9" s="72"/>
     </row>
     <row r="10" spans="1:8" ht="12.6" customHeight="1">
       <c r="A10" s="53">
@@ -2195,7 +2206,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="24"/>
-      <c r="H10" s="74"/>
+      <c r="H10" s="72"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="53">
@@ -2215,7 +2226,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="24"/>
-      <c r="H11" s="74"/>
+      <c r="H11" s="72"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="53">
@@ -2235,7 +2246,7 @@
         <v>4</v>
       </c>
       <c r="G12" s="24"/>
-      <c r="H12" s="74"/>
+      <c r="H12" s="72"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="53">
@@ -2255,7 +2266,7 @@
         <v>4</v>
       </c>
       <c r="G13" s="24"/>
-      <c r="H13" s="74"/>
+      <c r="H13" s="72"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="53">
@@ -2275,7 +2286,7 @@
         <v>4</v>
       </c>
       <c r="G14" s="24"/>
-      <c r="H14" s="74"/>
+      <c r="H14" s="72"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="53">
@@ -2295,7 +2306,7 @@
         <v>7</v>
       </c>
       <c r="G15" s="24"/>
-      <c r="H15" s="74"/>
+      <c r="H15" s="72"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="53">
@@ -2315,7 +2326,7 @@
         <v>7</v>
       </c>
       <c r="G16" s="24"/>
-      <c r="H16" s="74"/>
+      <c r="H16" s="72"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="53">
@@ -2335,7 +2346,7 @@
         <v>7</v>
       </c>
       <c r="G17" s="24"/>
-      <c r="H17" s="74"/>
+      <c r="H17" s="72"/>
     </row>
     <row r="18" spans="1:8" s="33" customFormat="1">
       <c r="A18" s="53">
@@ -2355,7 +2366,7 @@
         <v>7</v>
       </c>
       <c r="G18" s="32"/>
-      <c r="H18" s="81"/>
+      <c r="H18" s="79"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="53">
@@ -2375,7 +2386,7 @@
         <v>7</v>
       </c>
       <c r="G19" s="27"/>
-      <c r="H19" s="74"/>
+      <c r="H19" s="72"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="53">
@@ -2395,7 +2406,7 @@
         <v>7</v>
       </c>
       <c r="G20" s="27"/>
-      <c r="H20" s="74"/>
+      <c r="H20" s="72"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="53">
@@ -2415,7 +2426,7 @@
         <v>7</v>
       </c>
       <c r="G21" s="27"/>
-      <c r="H21" s="74"/>
+      <c r="H21" s="72"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="53">
@@ -2433,7 +2444,7 @@
       </c>
       <c r="F22" s="43"/>
       <c r="G22" s="27"/>
-      <c r="H22" s="74"/>
+      <c r="H22" s="72"/>
     </row>
     <row r="23" spans="1:8" ht="25.5">
       <c r="A23" s="53">
@@ -2451,7 +2462,7 @@
       </c>
       <c r="F23" s="44"/>
       <c r="G23" s="27"/>
-      <c r="H23" s="76"/>
+      <c r="H23" s="74"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="53">
@@ -2473,7 +2484,7 @@
         <v>7</v>
       </c>
       <c r="G24" s="27"/>
-      <c r="H24" s="74"/>
+      <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" s="33" customFormat="1" ht="25.5">
       <c r="A25" s="55">
@@ -2491,7 +2502,7 @@
       </c>
       <c r="F25" s="42"/>
       <c r="G25" s="40"/>
-      <c r="H25" s="81"/>
+      <c r="H25" s="79"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="53">
@@ -2509,7 +2520,7 @@
       </c>
       <c r="F26" s="43"/>
       <c r="G26" s="24"/>
-      <c r="H26" s="74"/>
+      <c r="H26" s="72"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="53">
@@ -2527,7 +2538,7 @@
       <c r="E27" s="19"/>
       <c r="F27" s="43"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="74"/>
+      <c r="H27" s="72"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="53">
@@ -2547,7 +2558,7 @@
         <v>7</v>
       </c>
       <c r="G28" s="24"/>
-      <c r="H28" s="74"/>
+      <c r="H28" s="72"/>
     </row>
     <row r="29" spans="1:8" ht="13.5" thickBot="1">
       <c r="A29" s="57">
@@ -2567,27 +2578,27 @@
         <v>7</v>
       </c>
       <c r="G29" s="62"/>
-      <c r="H29" s="78"/>
+      <c r="H29" s="76"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="53">
         <v>25</v>
       </c>
-      <c r="B30" s="70" t="s">
+      <c r="B30" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="87" t="s">
+      <c r="C30" s="85" t="s">
         <v>110</v>
       </c>
       <c r="D30" s="52" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="52"/>
-      <c r="F30" s="71">
+      <c r="F30" s="69">
         <v>3</v>
       </c>
-      <c r="G30" s="72"/>
-      <c r="H30" s="73"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="71"/>
     </row>
     <row r="31" spans="1:8" ht="13.5" thickBot="1">
       <c r="A31" s="57">
@@ -2607,7 +2618,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="27"/>
-      <c r="H31" s="74"/>
+      <c r="H31" s="72"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="53">
@@ -2627,13 +2638,13 @@
         <v>108</v>
       </c>
       <c r="G32" s="24"/>
-      <c r="H32" s="74"/>
+      <c r="H32" s="72"/>
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1">
       <c r="A33" s="57">
         <v>28</v>
       </c>
-      <c r="B33" s="75" t="s">
+      <c r="B33" s="73" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="18" t="s">
@@ -2647,13 +2658,13 @@
         <v>3</v>
       </c>
       <c r="G33" s="24"/>
-      <c r="H33" s="74"/>
+      <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:8" ht="15">
       <c r="A34" s="53">
         <v>29</v>
       </c>
-      <c r="B34" s="75" t="s">
+      <c r="B34" s="73" t="s">
         <v>70</v>
       </c>
       <c r="C34" s="18" t="s">
@@ -2667,7 +2678,7 @@
         <v>3.7</v>
       </c>
       <c r="G34" s="24"/>
-      <c r="H34" s="74"/>
+      <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:8" ht="13.5" thickBot="1">
       <c r="A35" s="57">
@@ -2685,7 +2696,7 @@
       <c r="E35" s="19"/>
       <c r="F35" s="24"/>
       <c r="G35" s="24"/>
-      <c r="H35" s="74"/>
+      <c r="H35" s="72"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="53">
@@ -2705,7 +2716,7 @@
         <v>9</v>
       </c>
       <c r="G36" s="24"/>
-      <c r="H36" s="76"/>
+      <c r="H36" s="74"/>
     </row>
     <row r="37" spans="1:8" ht="13.5" thickBot="1">
       <c r="A37" s="57">
@@ -2725,7 +2736,7 @@
         <v>9</v>
       </c>
       <c r="G37" s="24"/>
-      <c r="H37" s="74"/>
+      <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="53">
@@ -2745,7 +2756,7 @@
         <v>9</v>
       </c>
       <c r="G38" s="24"/>
-      <c r="H38" s="74"/>
+      <c r="H38" s="72"/>
     </row>
     <row r="39" spans="1:8" ht="13.5" thickBot="1">
       <c r="A39" s="57">
@@ -2765,7 +2776,7 @@
         <v>9</v>
       </c>
       <c r="G39" s="27"/>
-      <c r="H39" s="74"/>
+      <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="53">
@@ -2774,7 +2785,7 @@
       <c r="B40" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="86" t="s">
+      <c r="C40" s="84" t="s">
         <v>55</v>
       </c>
       <c r="D40" s="19" t="s">
@@ -2785,7 +2796,7 @@
       </c>
       <c r="F40" s="24"/>
       <c r="G40" s="24"/>
-      <c r="H40" s="74"/>
+      <c r="H40" s="72"/>
     </row>
     <row r="41" spans="1:8" ht="13.5" thickBot="1">
       <c r="A41" s="57">
@@ -2805,7 +2816,7 @@
         <v>9</v>
       </c>
       <c r="G41" s="24"/>
-      <c r="H41" s="74"/>
+      <c r="H41" s="72"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="53">
@@ -2825,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="G42" s="24"/>
-      <c r="H42" s="74"/>
+      <c r="H42" s="72"/>
     </row>
     <row r="43" spans="1:8" ht="13.5" thickBot="1">
       <c r="A43" s="57">
@@ -2845,13 +2856,13 @@
         <v>11</v>
       </c>
       <c r="G43" s="24"/>
-      <c r="H43" s="74"/>
+      <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" ht="13.5" thickBot="1">
       <c r="A44" s="53">
         <v>39</v>
       </c>
-      <c r="B44" s="77" t="s">
+      <c r="B44" s="75" t="s">
         <v>80</v>
       </c>
       <c r="C44" s="47" t="s">
@@ -2863,25 +2874,25 @@
       </c>
       <c r="F44" s="64"/>
       <c r="G44" s="64"/>
-      <c r="H44" s="78"/>
+      <c r="H44" s="76"/>
     </row>
     <row r="45" spans="1:8" ht="13.5" thickBot="1">
       <c r="A45" s="57">
         <v>40</v>
       </c>
-      <c r="B45" s="82" t="s">
+      <c r="B45" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="87" t="s">
+      <c r="C45" s="85" t="s">
         <v>110</v>
       </c>
       <c r="D45" s="52" t="s">
         <v>6</v>
       </c>
       <c r="E45" s="52"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="72"/>
-      <c r="H45" s="73"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="71"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="53">
@@ -2899,7 +2910,7 @@
       </c>
       <c r="F46" s="24"/>
       <c r="G46" s="24"/>
-      <c r="H46" s="74"/>
+      <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:8" ht="13.5" thickBot="1">
       <c r="A47" s="57">
@@ -2919,7 +2930,7 @@
         <v>12</v>
       </c>
       <c r="G47" s="24"/>
-      <c r="H47" s="74"/>
+      <c r="H47" s="72"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="53">
@@ -2928,7 +2939,7 @@
       <c r="B48" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C48" s="86" t="s">
+      <c r="C48" s="84" t="s">
         <v>55</v>
       </c>
       <c r="D48" s="19" t="s">
@@ -2937,7 +2948,7 @@
       <c r="E48" s="19"/>
       <c r="F48" s="24"/>
       <c r="G48" s="24"/>
-      <c r="H48" s="74"/>
+      <c r="H48" s="72"/>
     </row>
     <row r="49" spans="1:8" ht="13.5" thickBot="1">
       <c r="A49" s="57">
@@ -2957,7 +2968,7 @@
         <v>7</v>
       </c>
       <c r="G49" s="24"/>
-      <c r="H49" s="74"/>
+      <c r="H49" s="72"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="53">
@@ -2977,7 +2988,7 @@
         <v>7</v>
       </c>
       <c r="G50" s="24"/>
-      <c r="H50" s="74"/>
+      <c r="H50" s="72"/>
     </row>
     <row r="51" spans="1:8" ht="13.5" thickBot="1">
       <c r="A51" s="57">
@@ -2997,7 +3008,7 @@
         <v>11.1</v>
       </c>
       <c r="G51" s="24"/>
-      <c r="H51" s="74"/>
+      <c r="H51" s="72"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="53">
@@ -3012,12 +3023,12 @@
       <c r="D52" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E52" s="83"/>
-      <c r="F52" s="24">
-        <v>12</v>
+      <c r="E52" s="81"/>
+      <c r="F52" s="24" t="s">
+        <v>117</v>
       </c>
       <c r="G52" s="24"/>
-      <c r="H52" s="74"/>
+      <c r="H52" s="72"/>
     </row>
     <row r="53" spans="1:8" ht="13.5" thickBot="1">
       <c r="A53" s="57">
@@ -3033,31 +3044,31 @@
         <v>6</v>
       </c>
       <c r="E53" s="48"/>
-      <c r="F53" s="64">
-        <v>12</v>
+      <c r="F53" s="64" t="s">
+        <v>117</v>
       </c>
       <c r="G53" s="64"/>
-      <c r="H53" s="78"/>
+      <c r="H53" s="76"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="53">
         <v>49</v>
       </c>
-      <c r="B54" s="84" t="s">
+      <c r="B54" s="82" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="88" t="s">
+      <c r="C54" s="86" t="s">
         <v>55</v>
       </c>
       <c r="D54" s="52" t="s">
         <v>6</v>
       </c>
       <c r="E54" s="52"/>
-      <c r="F54" s="72">
+      <c r="F54" s="70">
         <v>1</v>
       </c>
-      <c r="G54" s="72"/>
-      <c r="H54" s="73"/>
+      <c r="G54" s="70"/>
+      <c r="H54" s="71"/>
     </row>
     <row r="55" spans="1:8" ht="13.5" thickBot="1">
       <c r="A55" s="57">
@@ -3066,7 +3077,7 @@
       <c r="B55" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="C55" s="86" t="s">
+      <c r="C55" s="84" t="s">
         <v>55</v>
       </c>
       <c r="D55" s="19" t="s">
@@ -3077,7 +3088,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="24"/>
-      <c r="H55" s="74"/>
+      <c r="H55" s="72"/>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="53">
@@ -3095,7 +3106,7 @@
       </c>
       <c r="F56" s="24"/>
       <c r="G56" s="24"/>
-      <c r="H56" s="74"/>
+      <c r="H56" s="72"/>
     </row>
     <row r="57" spans="1:8" ht="13.5" thickBot="1">
       <c r="A57" s="57">
@@ -3115,7 +3126,7 @@
         <v>2.7</v>
       </c>
       <c r="G57" s="24"/>
-      <c r="H57" s="74"/>
+      <c r="H57" s="72"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="53">
@@ -3124,7 +3135,7 @@
       <c r="B58" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="C58" s="86" t="s">
+      <c r="C58" s="84" t="s">
         <v>55</v>
       </c>
       <c r="D58" s="19" t="s">
@@ -3135,7 +3146,7 @@
         <v>8</v>
       </c>
       <c r="G58" s="24"/>
-      <c r="H58" s="74"/>
+      <c r="H58" s="72"/>
     </row>
     <row r="59" spans="1:8" ht="13.5" thickBot="1">
       <c r="A59" s="57">
@@ -3155,7 +3166,7 @@
         <v>7</v>
       </c>
       <c r="G59" s="24"/>
-      <c r="H59" s="74"/>
+      <c r="H59" s="72"/>
     </row>
     <row r="60" spans="1:8" ht="25.5">
       <c r="A60" s="53">
@@ -3175,7 +3186,7 @@
         <v>7</v>
       </c>
       <c r="G60" s="24"/>
-      <c r="H60" s="74"/>
+      <c r="H60" s="72"/>
     </row>
     <row r="61" spans="1:8" ht="26.25" thickBot="1">
       <c r="A61" s="57">
@@ -3197,7 +3208,7 @@
         <v>8</v>
       </c>
       <c r="G61" s="24"/>
-      <c r="H61" s="74"/>
+      <c r="H61" s="72"/>
     </row>
     <row r="62" spans="1:8" ht="25.5">
       <c r="A62" s="53">
@@ -3217,7 +3228,7 @@
         <v>2</v>
       </c>
       <c r="G62" s="24"/>
-      <c r="H62" s="74"/>
+      <c r="H62" s="72"/>
     </row>
     <row r="63" spans="1:8" ht="13.5" thickBot="1">
       <c r="A63" s="57">
@@ -3237,7 +3248,7 @@
         <v>14</v>
       </c>
       <c r="G63" s="24"/>
-      <c r="H63" s="74"/>
+      <c r="H63" s="72"/>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="53">
@@ -3255,7 +3266,7 @@
       <c r="E64" s="19"/>
       <c r="F64" s="24"/>
       <c r="G64" s="24"/>
-      <c r="H64" s="74"/>
+      <c r="H64" s="72"/>
     </row>
     <row r="65" spans="1:8" ht="13.5" thickBot="1">
       <c r="A65" s="57">
@@ -3277,7 +3288,7 @@
         <v>15</v>
       </c>
       <c r="G65" s="24"/>
-      <c r="H65" s="74"/>
+      <c r="H65" s="72"/>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="53">
@@ -3297,13 +3308,13 @@
         <v>2</v>
       </c>
       <c r="G66" s="24"/>
-      <c r="H66" s="74"/>
+      <c r="H66" s="72"/>
     </row>
     <row r="67" spans="1:8" ht="13.5" thickBot="1">
       <c r="A67" s="57">
         <v>62</v>
       </c>
-      <c r="B67" s="77" t="s">
+      <c r="B67" s="75" t="s">
         <v>45</v>
       </c>
       <c r="C67" s="47" t="s">
@@ -3317,25 +3328,25 @@
         <v>2</v>
       </c>
       <c r="G67" s="64"/>
-      <c r="H67" s="78"/>
+      <c r="H67" s="76"/>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="53">
         <v>63</v>
       </c>
-      <c r="B68" s="82" t="s">
+      <c r="B68" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="C68" s="87" t="s">
+      <c r="C68" s="85" t="s">
         <v>110</v>
       </c>
       <c r="D68" s="52"/>
       <c r="E68" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="F68" s="72"/>
-      <c r="G68" s="72"/>
-      <c r="H68" s="73"/>
+      <c r="F68" s="70"/>
+      <c r="G68" s="70"/>
+      <c r="H68" s="71"/>
     </row>
     <row r="69" spans="1:8" ht="13.5" thickBot="1">
       <c r="A69" s="57">
@@ -3353,7 +3364,7 @@
       </c>
       <c r="F69" s="24"/>
       <c r="G69" s="24"/>
-      <c r="H69" s="74"/>
+      <c r="H69" s="72"/>
     </row>
     <row r="70" spans="1:8" ht="25.5">
       <c r="A70" s="53">
@@ -3371,7 +3382,7 @@
       </c>
       <c r="F70" s="24"/>
       <c r="G70" s="24"/>
-      <c r="H70" s="74"/>
+      <c r="H70" s="72"/>
     </row>
     <row r="71" spans="1:8" ht="26.25" thickBot="1">
       <c r="A71" s="57">
@@ -3389,7 +3400,7 @@
       </c>
       <c r="F71" s="24"/>
       <c r="G71" s="24"/>
-      <c r="H71" s="74"/>
+      <c r="H71" s="72"/>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="53">
@@ -3407,7 +3418,7 @@
       </c>
       <c r="F72" s="24"/>
       <c r="G72" s="24"/>
-      <c r="H72" s="74"/>
+      <c r="H72" s="72"/>
     </row>
     <row r="73" spans="1:8" ht="13.5" thickBot="1">
       <c r="A73" s="57">
@@ -3425,7 +3436,7 @@
       </c>
       <c r="F73" s="24"/>
       <c r="G73" s="24"/>
-      <c r="H73" s="74"/>
+      <c r="H73" s="72"/>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="53">
@@ -3443,13 +3454,13 @@
       </c>
       <c r="F74" s="24"/>
       <c r="G74" s="24"/>
-      <c r="H74" s="74"/>
+      <c r="H74" s="72"/>
     </row>
     <row r="75" spans="1:8" ht="13.5" thickBot="1">
       <c r="A75" s="57">
         <v>70</v>
       </c>
-      <c r="B75" s="85" t="s">
+      <c r="B75" s="83" t="s">
         <v>106</v>
       </c>
       <c r="C75" s="47" t="s">
@@ -3461,16 +3472,16 @@
       </c>
       <c r="F75" s="64"/>
       <c r="G75" s="64"/>
-      <c r="H75" s="78"/>
+      <c r="H75" s="76"/>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="68" t="s">
+      <c r="A76" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="B76" s="101" t="s">
+      <c r="B76" s="87" t="s">
         <v>111</v>
       </c>
-      <c r="C76" s="69" t="s">
+      <c r="C76" s="67" t="s">
         <v>55</v>
       </c>
       <c r="D76" s="45" t="s">
@@ -3484,13 +3495,13 @@
       <c r="H76" s="59"/>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" s="102" t="s">
+      <c r="A77" s="88" t="s">
         <v>114</v>
       </c>
       <c r="B77" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="C77" s="103" t="s">
+      <c r="C77" s="89" t="s">
         <v>55</v>
       </c>
       <c r="D77" s="19" t="s">
@@ -3503,37 +3514,58 @@
       <c r="G77" s="24"/>
       <c r="H77" s="24"/>
     </row>
-    <row r="78" spans="1:8">
-      <c r="A78" s="66"/>
-      <c r="B78" s="21"/>
-      <c r="C78" s="67"/>
-      <c r="D78" s="19"/>
-      <c r="E78" s="19"/>
-      <c r="F78" s="24"/>
-      <c r="G78" s="24"/>
-      <c r="H78" s="24"/>
-    </row>
-    <row r="79" spans="1:8">
-      <c r="A79" s="66"/>
-      <c r="B79" s="21"/>
-      <c r="C79" s="67"/>
-      <c r="D79" s="19"/>
-      <c r="E79" s="19"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="24"/>
-      <c r="H79" s="24"/>
-    </row>
-    <row r="80" spans="1:8">
-      <c r="A80" s="66"/>
-      <c r="B80" s="21"/>
-      <c r="C80" s="67"/>
-      <c r="D80" s="19"/>
-      <c r="E80" s="19"/>
-      <c r="F80" s="24"/>
-      <c r="G80" s="24"/>
-      <c r="H80" s="24"/>
+    <row r="78" spans="1:8" s="106" customFormat="1">
+      <c r="A78" s="102"/>
+      <c r="B78" s="103"/>
+      <c r="C78" s="104"/>
+      <c r="D78" s="81"/>
+      <c r="E78" s="81"/>
+      <c r="F78" s="105"/>
+      <c r="G78" s="105"/>
+      <c r="H78" s="105"/>
+    </row>
+    <row r="79" spans="1:8" s="106" customFormat="1">
+      <c r="A79" s="102"/>
+      <c r="B79" s="103"/>
+      <c r="C79" s="104"/>
+      <c r="D79" s="81"/>
+      <c r="E79" s="81"/>
+      <c r="F79" s="105"/>
+      <c r="G79" s="105"/>
+      <c r="H79" s="105"/>
+    </row>
+    <row r="80" spans="1:8" s="106" customFormat="1">
+      <c r="A80" s="102"/>
+      <c r="B80" s="103"/>
+      <c r="C80" s="104"/>
+      <c r="D80" s="81"/>
+      <c r="E80" s="81"/>
+      <c r="F80" s="105"/>
+      <c r="G80" s="105"/>
+      <c r="H80" s="105"/>
+    </row>
+    <row r="81" spans="1:8" s="106" customFormat="1">
+      <c r="A81" s="102"/>
+      <c r="B81" s="103"/>
+      <c r="C81" s="104"/>
+      <c r="D81" s="81"/>
+      <c r="E81" s="81"/>
+      <c r="F81" s="105"/>
+      <c r="G81" s="105"/>
+      <c r="H81" s="105"/>
+    </row>
+    <row r="82" spans="1:8" s="106" customFormat="1">
+      <c r="A82" s="102"/>
+      <c r="B82" s="103"/>
+      <c r="C82" s="104"/>
+      <c r="D82" s="81"/>
+      <c r="E82" s="81"/>
+      <c r="F82" s="105"/>
+      <c r="G82" s="105"/>
+      <c r="H82" s="105"/>
     </row>
   </sheetData>
+  <autoFilter ref="F1:F80" xr:uid="{4A3DAA3C-C6B7-4DE2-BF03-29C3D6359CDF}"/>
   <mergeCells count="6">
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="C1:D2"/>
@@ -3552,7 +3584,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="66" fitToHeight="8" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="87" fitToHeight="8" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
UC Graph and UC-Spec
</commit_message>
<xml_diff>
--- a/Docs/Requirements-Table.xlsx
+++ b/Docs/Requirements-Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Terkel\OneDrive\Study\SE\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Terkel\OneDrive\Study\SE\git\segroup9\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E315C0-FA9A-4A1F-B895-7EF5B03B4CDF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE70CE8D-F474-4FD3-B504-0BAEB145B5B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="סוגי דרישות" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">דרישות!$F$1:$F$80</definedName>
     <definedName name="FR">'סוגי דרישות'!$B$5:$B$6</definedName>
     <definedName name="FuncReq">'סוגי דרישות'!$B$5:$B$6</definedName>
     <definedName name="HML">'סוגי דרישות'!#REF!</definedName>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="118">
   <si>
     <t>זיהוי</t>
   </si>
@@ -232,9 +233,6 @@
     <t>אותה משתמשת לא יכולה להיות מחוברת למערכת בו זמנית יותר מפעם אחת</t>
   </si>
   <si>
-    <t>ליל הינה מערכת ממוחשבת המאפשרת ללקוחות לעיין בקטלוג לבחור פריטים ולהזמין משלוח</t>
-  </si>
-  <si>
     <t>לקוחה יכולה ליצור הזמנה דרך האינטרנט</t>
   </si>
   <si>
@@ -288,13 +286,7 @@
     </r>
   </si>
   <si>
-    <t>בהגדרה עצית ניתן לבחור סוג פריט</t>
-  </si>
-  <si>
     <t>בהגדרה עצית ניתן לבחור צבע שולט</t>
-  </si>
-  <si>
-    <t>בהגדרה עצית ניתן לבחור טווח מחירים</t>
   </si>
   <si>
     <r>
@@ -887,6 +879,39 @@
   </si>
   <si>
     <t>התקשורת בין התחנות לשרת המערכת תפעל רק דרך רשת מקומית (LAN TCP\IP)</t>
+  </si>
+  <si>
+    <t>לילך הינה מערכת ממוחשבת המאפשרת ללקוחות לעיין בקטלוג לבחור פריטים ולהזמין משלוח</t>
+  </si>
+  <si>
+    <t>13,3,6</t>
+  </si>
+  <si>
+    <t>מנהל יכול לצפות בנתוני עובדים</t>
+  </si>
+  <si>
+    <t>סיפור לקוח</t>
+  </si>
+  <si>
+    <t>יכולת חיפוש בקטלוג</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>יכולת טיפול בתלונה</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>בהגדרה עצית יש לבחור סוג פריט</t>
+  </si>
+  <si>
+    <t>בהגדרה עצית יש לבחור טווח מחירים</t>
+  </si>
+  <si>
+    <t>12, 16</t>
   </si>
 </sst>
 </file>
@@ -1041,7 +1066,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1341,24 +1366,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -1464,49 +1476,10 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1523,9 +1496,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1585,20 +1555,8 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="2"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="2"/>
@@ -1622,18 +1580,9 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1646,33 +1595,85 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2014,11 +2015,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
+      <pane ySplit="5" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2040,10 +2041,10 @@
       <c r="B1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="43"/>
+      <c r="D1" s="94"/>
       <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1">
@@ -2053,8 +2054,8 @@
       <c r="B2" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="94"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="1"/>
@@ -2072,346 +2073,406 @@
       <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="39" t="s">
+      <c r="E4" s="92"/>
+      <c r="F4" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="41"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="92"/>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A5" s="48"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="50"/>
+      <c r="A5" s="99"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="101"/>
       <c r="D5" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="98" t="s">
+      <c r="F5" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="98" t="s">
+      <c r="G5" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="98" t="s">
+      <c r="H5" s="77" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="25.5">
-      <c r="A6" s="64">
+      <c r="A6" s="50">
         <v>1</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="52"/>
+      <c r="E6" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="78"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="71"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="53">
+        <v>2</v>
+      </c>
+      <c r="B7" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="60" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="99"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="89"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="67">
-        <v>2</v>
-      </c>
-      <c r="B7" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="18"/>
+      <c r="C7" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D7" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="20"/>
-      <c r="F7" s="56"/>
+      <c r="F7" s="43">
+        <v>5</v>
+      </c>
       <c r="G7" s="24"/>
-      <c r="H7" s="90"/>
+      <c r="H7" s="72"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
-      <c r="A8" s="67">
+      <c r="A8" s="53">
         <v>3</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="18"/>
+        <v>47</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D8" s="19"/>
       <c r="E8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="56"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="24"/>
-      <c r="H8" s="90"/>
+      <c r="H8" s="72"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="67">
+      <c r="A9" s="53">
         <v>4</v>
       </c>
       <c r="B9" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D9" s="19"/>
       <c r="E9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="56"/>
+      <c r="F9" s="43">
+        <v>5</v>
+      </c>
       <c r="G9" s="24"/>
-      <c r="H9" s="90"/>
+      <c r="H9" s="72"/>
     </row>
     <row r="10" spans="1:8" ht="12.6" customHeight="1">
-      <c r="A10" s="67">
+      <c r="A10" s="53">
         <v>5</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="18"/>
+        <v>48</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D10" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="20"/>
-      <c r="F10" s="56"/>
+      <c r="F10" s="43">
+        <v>3</v>
+      </c>
       <c r="G10" s="24"/>
-      <c r="H10" s="90"/>
+      <c r="H10" s="72"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="67">
+      <c r="A11" s="53">
         <v>6</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="18"/>
+        <v>49</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D11" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="20"/>
-      <c r="F11" s="63"/>
+      <c r="F11" s="49">
+        <v>4</v>
+      </c>
       <c r="G11" s="24"/>
-      <c r="H11" s="90"/>
+      <c r="H11" s="72"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="67">
+      <c r="A12" s="53">
         <v>7</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="18"/>
+        <v>115</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D12" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="20"/>
-      <c r="F12" s="56"/>
+      <c r="F12" s="43">
+        <v>4</v>
+      </c>
       <c r="G12" s="24"/>
-      <c r="H12" s="90"/>
+      <c r="H12" s="72"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="67">
+      <c r="A13" s="53">
         <v>8</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="18"/>
+        <v>50</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D13" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="20"/>
-      <c r="F13" s="56"/>
+      <c r="F13" s="43">
+        <v>4</v>
+      </c>
       <c r="G13" s="24"/>
-      <c r="H13" s="90"/>
+      <c r="H13" s="72"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="67">
+      <c r="A14" s="53">
         <v>9</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="18"/>
+        <v>116</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D14" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="19"/>
-      <c r="F14" s="56"/>
+      <c r="F14" s="43">
+        <v>4</v>
+      </c>
       <c r="G14" s="24"/>
-      <c r="H14" s="90"/>
+      <c r="H14" s="72"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="67">
+      <c r="A15" s="53">
         <v>10</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="18"/>
+        <v>51</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D15" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="19"/>
-      <c r="F15" s="63"/>
+      <c r="F15" s="49">
+        <v>7</v>
+      </c>
       <c r="G15" s="24"/>
-      <c r="H15" s="90"/>
+      <c r="H15" s="72"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="67">
+      <c r="A16" s="53">
         <v>11</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="18"/>
+        <v>52</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D16" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="19"/>
-      <c r="F16" s="56"/>
+      <c r="F16" s="43">
+        <v>7</v>
+      </c>
       <c r="G16" s="24"/>
-      <c r="H16" s="90"/>
+      <c r="H16" s="72"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="67">
+      <c r="A17" s="53">
         <v>12</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="18"/>
+        <v>53</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D17" s="19"/>
       <c r="E17" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="56"/>
+      <c r="F17" s="43">
+        <v>7</v>
+      </c>
       <c r="G17" s="24"/>
-      <c r="H17" s="90"/>
+      <c r="H17" s="72"/>
     </row>
     <row r="18" spans="1:8" s="33" customFormat="1">
-      <c r="A18" s="67">
+      <c r="A18" s="53">
         <v>13</v>
       </c>
-      <c r="B18" s="51" t="s">
-        <v>57</v>
+      <c r="B18" s="39" t="s">
+        <v>54</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="20"/>
-      <c r="F18" s="55"/>
+      <c r="F18" s="42">
+        <v>7</v>
+      </c>
       <c r="G18" s="32"/>
-      <c r="H18" s="100"/>
+      <c r="H18" s="79"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="67">
+      <c r="A19" s="53">
         <v>14</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="18"/>
+        <v>58</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D19" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="19"/>
-      <c r="F19" s="56"/>
+      <c r="F19" s="43">
+        <v>7</v>
+      </c>
       <c r="G19" s="27"/>
-      <c r="H19" s="90"/>
+      <c r="H19" s="72"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="67">
+      <c r="A20" s="53">
         <v>15</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="18"/>
+        <v>56</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D20" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E20" s="19"/>
-      <c r="F20" s="56"/>
+      <c r="F20" s="43">
+        <v>7</v>
+      </c>
       <c r="G20" s="27"/>
-      <c r="H20" s="90"/>
+      <c r="H20" s="72"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="67">
+      <c r="A21" s="53">
         <v>16</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="18"/>
+        <v>57</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D21" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E21" s="19"/>
-      <c r="F21" s="56"/>
+      <c r="F21" s="43">
+        <v>7</v>
+      </c>
       <c r="G21" s="27"/>
-      <c r="H21" s="90"/>
+      <c r="H21" s="72"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="67">
+      <c r="A22" s="53">
         <v>17</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="18"/>
+        <v>59</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D22" s="19"/>
       <c r="E22" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="56"/>
+      <c r="F22" s="43"/>
       <c r="G22" s="27"/>
-      <c r="H22" s="90"/>
+      <c r="H22" s="72"/>
     </row>
     <row r="23" spans="1:8" ht="25.5">
-      <c r="A23" s="67">
+      <c r="A23" s="53">
         <v>18</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="19" t="s">
-        <v>6</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="19"/>
       <c r="E23" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="57"/>
+      <c r="F23" s="44"/>
       <c r="G23" s="27"/>
-      <c r="H23" s="92"/>
+      <c r="H23" s="74"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="67">
+      <c r="A24" s="53">
         <v>19</v>
       </c>
-      <c r="B24" s="54" t="s">
-        <v>64</v>
+      <c r="B24" s="41" t="s">
+        <v>61</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>6</v>
@@ -2419,239 +2480,313 @@
       <c r="E24" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="56"/>
+      <c r="F24" s="43">
+        <v>7</v>
+      </c>
       <c r="G24" s="27"/>
-      <c r="H24" s="90"/>
+      <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" s="33" customFormat="1" ht="25.5">
-      <c r="A25" s="69">
+      <c r="A25" s="55">
         <v>20</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="52"/>
+        <v>62</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="55"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="100"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="79"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="67">
+      <c r="A26" s="53">
         <v>21</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="18"/>
+        <v>63</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D26" s="19"/>
       <c r="E26" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="56"/>
+      <c r="F26" s="43"/>
       <c r="G26" s="24"/>
-      <c r="H26" s="90"/>
+      <c r="H26" s="72"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="67">
+      <c r="A27" s="53">
         <v>22</v>
       </c>
-      <c r="B27" s="70" t="s">
-        <v>67</v>
+      <c r="B27" s="56" t="s">
+        <v>64</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="19"/>
-      <c r="F27" s="56"/>
+      <c r="F27" s="43"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="90"/>
+      <c r="H27" s="72"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="67">
+      <c r="A28" s="53">
         <v>23</v>
       </c>
       <c r="B28" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="18"/>
+      <c r="C28" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D28" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="19"/>
-      <c r="F28" s="24"/>
+      <c r="F28" s="24">
+        <v>7</v>
+      </c>
       <c r="G28" s="24"/>
-      <c r="H28" s="90"/>
+      <c r="H28" s="72"/>
     </row>
     <row r="29" spans="1:8" ht="13.5" thickBot="1">
-      <c r="A29" s="71">
+      <c r="A29" s="57">
         <v>24</v>
       </c>
-      <c r="B29" s="72" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="61"/>
-      <c r="D29" s="77" t="s">
+      <c r="B29" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="74"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="76"/>
-      <c r="H29" s="97"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="61">
+        <v>7</v>
+      </c>
+      <c r="G29" s="62"/>
+      <c r="H29" s="76"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="64"/>
-      <c r="B30" s="86" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="59"/>
-      <c r="D30" s="66" t="s">
+      <c r="A30" s="53">
+        <v>25</v>
+      </c>
+      <c r="B30" s="68" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="85" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="88"/>
-      <c r="H30" s="89"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="67"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="69">
+        <v>3</v>
+      </c>
+      <c r="G30" s="70"/>
+      <c r="H30" s="71"/>
+    </row>
+    <row r="31" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A31" s="57">
+        <v>26</v>
+      </c>
       <c r="B31" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D31" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="19"/>
-      <c r="F31" s="25"/>
+      <c r="F31" s="25">
+        <v>3</v>
+      </c>
       <c r="G31" s="27"/>
-      <c r="H31" s="90"/>
+      <c r="H31" s="72"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="67"/>
+      <c r="A32" s="53">
+        <v>27</v>
+      </c>
       <c r="B32" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="18"/>
+        <v>68</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D32" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E32" s="19"/>
-      <c r="F32" s="24"/>
+      <c r="F32" s="24" t="s">
+        <v>108</v>
+      </c>
       <c r="G32" s="24"/>
-      <c r="H32" s="90"/>
-    </row>
-    <row r="33" spans="1:8" ht="14.25">
-      <c r="A33" s="67"/>
-      <c r="B33" s="91" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="18"/>
+      <c r="H32" s="72"/>
+    </row>
+    <row r="33" spans="1:8" ht="15" thickBot="1">
+      <c r="A33" s="57">
+        <v>28</v>
+      </c>
+      <c r="B33" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D33" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E33" s="19"/>
-      <c r="F33" s="24"/>
+      <c r="F33" s="24">
+        <v>3</v>
+      </c>
       <c r="G33" s="24"/>
-      <c r="H33" s="90"/>
+      <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:8" ht="15">
-      <c r="A34" s="67"/>
-      <c r="B34" s="91" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="18"/>
+      <c r="A34" s="53">
+        <v>29</v>
+      </c>
+      <c r="B34" s="73" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D34" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E34" s="19"/>
-      <c r="F34" s="24"/>
+      <c r="F34" s="24">
+        <v>3.7</v>
+      </c>
       <c r="G34" s="24"/>
-      <c r="H34" s="90"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="67"/>
+      <c r="H34" s="72"/>
+    </row>
+    <row r="35" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A35" s="57">
+        <v>30</v>
+      </c>
       <c r="B35" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D35" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E35" s="19"/>
       <c r="F35" s="24"/>
       <c r="G35" s="24"/>
-      <c r="H35" s="90"/>
+      <c r="H35" s="72"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="67"/>
-      <c r="B36" s="79" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="18"/>
+      <c r="A36" s="53">
+        <v>31</v>
+      </c>
+      <c r="B36" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D36" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E36" s="19"/>
-      <c r="F36" s="28"/>
+      <c r="F36" s="28">
+        <v>9</v>
+      </c>
       <c r="G36" s="24"/>
-      <c r="H36" s="92"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="67"/>
+      <c r="H36" s="74"/>
+    </row>
+    <row r="37" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A37" s="57">
+        <v>32</v>
+      </c>
       <c r="B37" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="18"/>
+        <v>73</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D37" s="19"/>
       <c r="E37" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F37" s="24"/>
+      <c r="F37" s="24">
+        <v>9</v>
+      </c>
       <c r="G37" s="24"/>
-      <c r="H37" s="90"/>
+      <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="67"/>
+      <c r="A38" s="53">
+        <v>33</v>
+      </c>
       <c r="B38" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" s="18"/>
+        <v>74</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F38" s="26"/>
+      <c r="F38" s="26">
+        <v>9</v>
+      </c>
       <c r="G38" s="24"/>
-      <c r="H38" s="90"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="67"/>
+      <c r="H38" s="72"/>
+    </row>
+    <row r="39" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A39" s="57">
+        <v>34</v>
+      </c>
       <c r="B39" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" s="18"/>
+        <v>75</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D39" s="19"/>
       <c r="E39" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F39" s="24"/>
+      <c r="F39" s="24">
+        <v>9</v>
+      </c>
       <c r="G39" s="27"/>
-      <c r="H39" s="90"/>
+      <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="93"/>
-      <c r="B40" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="C40" s="82" t="s">
-        <v>58</v>
+      <c r="A40" s="53">
+        <v>35</v>
+      </c>
+      <c r="B40" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="84" t="s">
+        <v>55</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>6</v>
@@ -2661,113 +2796,151 @@
       </c>
       <c r="F40" s="24"/>
       <c r="G40" s="24"/>
-      <c r="H40" s="90"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="93"/>
+      <c r="H40" s="72"/>
+    </row>
+    <row r="41" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A41" s="57">
+        <v>36</v>
+      </c>
       <c r="B41" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="81"/>
+        <v>77</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D41" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E41" s="19"/>
-      <c r="F41" s="24"/>
+      <c r="F41" s="24">
+        <v>9</v>
+      </c>
       <c r="G41" s="24"/>
-      <c r="H41" s="90"/>
+      <c r="H41" s="72"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="93"/>
+      <c r="A42" s="53">
+        <v>37</v>
+      </c>
       <c r="B42" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="81"/>
+        <v>78</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D42" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E42" s="19"/>
-      <c r="F42" s="24"/>
+      <c r="F42" s="24">
+        <v>10</v>
+      </c>
       <c r="G42" s="24"/>
-      <c r="H42" s="90"/>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="93"/>
+      <c r="H42" s="72"/>
+    </row>
+    <row r="43" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A43" s="57">
+        <v>38</v>
+      </c>
       <c r="B43" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="C43" s="81"/>
+        <v>79</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D43" s="19"/>
       <c r="E43" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F43" s="24"/>
+      <c r="F43" s="24">
+        <v>11</v>
+      </c>
       <c r="G43" s="24"/>
-      <c r="H43" s="90"/>
+      <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" ht="13.5" thickBot="1">
-      <c r="A44" s="94"/>
-      <c r="B44" s="95" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" s="96"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="62" t="s">
+      <c r="A44" s="53">
+        <v>39</v>
+      </c>
+      <c r="B44" s="75" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="48"/>
+      <c r="E44" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="F44" s="78"/>
-      <c r="G44" s="78"/>
-      <c r="H44" s="97"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="101"/>
-      <c r="B45" s="102" t="s">
+      <c r="F44" s="64"/>
+      <c r="G44" s="64"/>
+      <c r="H44" s="76"/>
+    </row>
+    <row r="45" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A45" s="57">
+        <v>40</v>
+      </c>
+      <c r="B45" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="103"/>
-      <c r="D45" s="66" t="s">
+      <c r="C45" s="85" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="E45" s="66"/>
-      <c r="F45" s="88"/>
-      <c r="G45" s="88"/>
-      <c r="H45" s="89"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="71"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="93"/>
+      <c r="A46" s="53">
+        <v>41</v>
+      </c>
       <c r="B46" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" s="81"/>
+        <v>81</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D46" s="19"/>
       <c r="E46" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F46" s="24"/>
       <c r="G46" s="24"/>
-      <c r="H46" s="90"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="93"/>
+      <c r="H46" s="72"/>
+    </row>
+    <row r="47" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A47" s="57">
+        <v>42</v>
+      </c>
       <c r="B47" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C47" s="81"/>
+      <c r="C47" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D47" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E47" s="19"/>
-      <c r="F47" s="24"/>
+      <c r="F47" s="24">
+        <v>12</v>
+      </c>
       <c r="G47" s="24"/>
-      <c r="H47" s="90"/>
+      <c r="H47" s="72"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="93"/>
-      <c r="B48" s="79" t="s">
-        <v>85</v>
-      </c>
-      <c r="C48" s="82" t="s">
-        <v>58</v>
+      <c r="A48" s="53">
+        <v>43</v>
+      </c>
+      <c r="B48" s="65" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="84" t="s">
+        <v>55</v>
       </c>
       <c r="D48" s="19" t="s">
         <v>10</v>
@@ -2775,433 +2948,624 @@
       <c r="E48" s="19"/>
       <c r="F48" s="24"/>
       <c r="G48" s="24"/>
-      <c r="H48" s="90"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="93"/>
+      <c r="H48" s="72"/>
+    </row>
+    <row r="49" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A49" s="57">
+        <v>44</v>
+      </c>
       <c r="B49" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="C49" s="81"/>
+        <v>83</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D49" s="19"/>
       <c r="E49" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F49" s="24"/>
+      <c r="F49" s="24">
+        <v>7</v>
+      </c>
       <c r="G49" s="24"/>
-      <c r="H49" s="90"/>
+      <c r="H49" s="72"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="93"/>
+      <c r="A50" s="53">
+        <v>45</v>
+      </c>
       <c r="B50" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="C50" s="81"/>
+        <v>84</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D50" s="19"/>
       <c r="E50" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F50" s="24"/>
+      <c r="F50" s="24">
+        <v>7</v>
+      </c>
       <c r="G50" s="24"/>
-      <c r="H50" s="90"/>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="93"/>
+      <c r="H50" s="72"/>
+    </row>
+    <row r="51" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A51" s="57">
+        <v>46</v>
+      </c>
       <c r="B51" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="C51" s="81"/>
+        <v>85</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D51" s="19"/>
       <c r="E51" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F51" s="24"/>
+      <c r="F51" s="24">
+        <v>11.1</v>
+      </c>
       <c r="G51" s="24"/>
-      <c r="H51" s="90"/>
+      <c r="H51" s="72"/>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="93"/>
+      <c r="A52" s="53">
+        <v>47</v>
+      </c>
       <c r="B52" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="81"/>
+        <v>86</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D52" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E52" s="104"/>
-      <c r="F52" s="24"/>
+      <c r="E52" s="81"/>
+      <c r="F52" s="24" t="s">
+        <v>117</v>
+      </c>
       <c r="G52" s="24"/>
-      <c r="H52" s="90"/>
+      <c r="H52" s="72"/>
     </row>
     <row r="53" spans="1:8" ht="13.5" thickBot="1">
-      <c r="A53" s="94"/>
-      <c r="B53" s="72" t="s">
+      <c r="A53" s="57">
+        <v>48</v>
+      </c>
+      <c r="B53" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="48"/>
+      <c r="F53" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G53" s="64"/>
+      <c r="H53" s="76"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="53">
+        <v>49</v>
+      </c>
+      <c r="B54" s="82" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="86" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="52"/>
+      <c r="F54" s="70">
+        <v>1</v>
+      </c>
+      <c r="G54" s="70"/>
+      <c r="H54" s="71"/>
+    </row>
+    <row r="55" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A55" s="57">
+        <v>50</v>
+      </c>
+      <c r="B55" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="96"/>
-      <c r="D53" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="62"/>
-      <c r="F53" s="78"/>
-      <c r="G53" s="78"/>
-      <c r="H53" s="97"/>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="101"/>
-      <c r="B54" s="105" t="s">
-        <v>91</v>
-      </c>
-      <c r="C54" s="106" t="s">
-        <v>58</v>
-      </c>
-      <c r="D54" s="66" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="66"/>
-      <c r="F54" s="88"/>
-      <c r="G54" s="88"/>
-      <c r="H54" s="89"/>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="107"/>
-      <c r="B55" s="79" t="s">
-        <v>93</v>
-      </c>
-      <c r="C55" s="82" t="s">
-        <v>58</v>
+      <c r="C55" s="84" t="s">
+        <v>55</v>
       </c>
       <c r="D55" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E55" s="19"/>
-      <c r="F55" s="24"/>
+      <c r="F55" s="24">
+        <v>1</v>
+      </c>
       <c r="G55" s="24"/>
-      <c r="H55" s="90"/>
+      <c r="H55" s="72"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="108"/>
+      <c r="A56" s="53">
+        <v>51</v>
+      </c>
       <c r="B56" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="C56" s="81"/>
+        <v>89</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D56" s="19"/>
       <c r="E56" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F56" s="24"/>
       <c r="G56" s="24"/>
-      <c r="H56" s="90"/>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="108"/>
+      <c r="H56" s="72"/>
+    </row>
+    <row r="57" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A57" s="57">
+        <v>52</v>
+      </c>
       <c r="B57" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57" s="81"/>
+        <v>91</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D57" s="19"/>
       <c r="E57" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F57" s="24"/>
+      <c r="F57" s="24">
+        <v>2.7</v>
+      </c>
       <c r="G57" s="24"/>
-      <c r="H57" s="90"/>
+      <c r="H57" s="72"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="108"/>
-      <c r="B58" s="79" t="s">
-        <v>95</v>
-      </c>
-      <c r="C58" s="82" t="s">
-        <v>58</v>
+      <c r="A58" s="53">
+        <v>53</v>
+      </c>
+      <c r="B58" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" s="84" t="s">
+        <v>55</v>
       </c>
       <c r="D58" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E58" s="19"/>
-      <c r="F58" s="24"/>
+      <c r="F58" s="24">
+        <v>8</v>
+      </c>
       <c r="G58" s="24"/>
-      <c r="H58" s="90"/>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="93"/>
+      <c r="H58" s="72"/>
+    </row>
+    <row r="59" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A59" s="57">
+        <v>54</v>
+      </c>
       <c r="B59" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59" s="81"/>
+        <v>93</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D59" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E59" s="19"/>
-      <c r="F59" s="24"/>
+      <c r="F59" s="24">
+        <v>7</v>
+      </c>
       <c r="G59" s="24"/>
-      <c r="H59" s="90"/>
+      <c r="H59" s="72"/>
     </row>
     <row r="60" spans="1:8" ht="25.5">
-      <c r="A60" s="93"/>
+      <c r="A60" s="53">
+        <v>55</v>
+      </c>
       <c r="B60" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" s="81"/>
+        <v>94</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D60" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E60" s="19"/>
-      <c r="F60" s="24"/>
+      <c r="F60" s="24">
+        <v>7</v>
+      </c>
       <c r="G60" s="24"/>
-      <c r="H60" s="90"/>
-    </row>
-    <row r="61" spans="1:8" ht="25.5">
-      <c r="A61" s="93"/>
+      <c r="H60" s="72"/>
+    </row>
+    <row r="61" spans="1:8" ht="26.25" thickBot="1">
+      <c r="A61" s="57">
+        <v>56</v>
+      </c>
       <c r="B61" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C61" s="81"/>
+      <c r="C61" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D61" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E61" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F61" s="24"/>
+      <c r="F61" s="24">
+        <v>8</v>
+      </c>
       <c r="G61" s="24"/>
-      <c r="H61" s="90"/>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="93"/>
+      <c r="H61" s="72"/>
+    </row>
+    <row r="62" spans="1:8" ht="25.5">
+      <c r="A62" s="53">
+        <v>57</v>
+      </c>
       <c r="B62" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="C62" s="81"/>
+        <v>95</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D62" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E62" s="19"/>
-      <c r="F62" s="24"/>
+      <c r="F62" s="24">
+        <v>2</v>
+      </c>
       <c r="G62" s="24"/>
-      <c r="H62" s="90"/>
-    </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="93"/>
-      <c r="B63" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C63" s="81"/>
+      <c r="H62" s="72"/>
+    </row>
+    <row r="63" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A63" s="57">
+        <v>58</v>
+      </c>
+      <c r="B63" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D63" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="19"/>
+      <c r="F63" s="24">
+        <v>14</v>
+      </c>
+      <c r="G63" s="24"/>
+      <c r="H63" s="72"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="53">
+        <v>59</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E63" s="19"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="24"/>
-      <c r="H63" s="90"/>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="93"/>
-      <c r="B64" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C64" s="81"/>
-      <c r="D64" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E64" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="E64" s="19"/>
       <c r="F64" s="24"/>
       <c r="G64" s="24"/>
-      <c r="H64" s="90"/>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="93"/>
+      <c r="H64" s="72"/>
+    </row>
+    <row r="65" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A65" s="57">
+        <v>60</v>
+      </c>
       <c r="B65" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="C65" s="81"/>
-      <c r="D65" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D65" s="19" t="s">
+        <v>6</v>
+      </c>
       <c r="E65" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F65" s="24">
+        <v>15</v>
+      </c>
+      <c r="G65" s="24"/>
+      <c r="H65" s="72"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="53">
+        <v>61</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F65" s="24"/>
-      <c r="G65" s="24"/>
-      <c r="H65" s="90"/>
-    </row>
-    <row r="66" spans="1:8" ht="13.5" thickBot="1">
-      <c r="A66" s="94"/>
-      <c r="B66" s="95" t="s">
+      <c r="F66" s="24">
+        <v>2</v>
+      </c>
+      <c r="G66" s="24"/>
+      <c r="H66" s="72"/>
+    </row>
+    <row r="67" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A67" s="57">
+        <v>62</v>
+      </c>
+      <c r="B67" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="C66" s="96"/>
-      <c r="D66" s="62"/>
-      <c r="E66" s="62" t="s">
+      <c r="C67" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" s="48"/>
+      <c r="E67" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="F66" s="78"/>
-      <c r="G66" s="78"/>
-      <c r="H66" s="97"/>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="101"/>
-      <c r="B67" s="102" t="s">
-        <v>102</v>
-      </c>
-      <c r="C67" s="103"/>
-      <c r="D67" s="66"/>
-      <c r="E67" s="66" t="s">
+      <c r="F67" s="64">
+        <v>2</v>
+      </c>
+      <c r="G67" s="64"/>
+      <c r="H67" s="76"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="53">
+        <v>63</v>
+      </c>
+      <c r="B68" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="C68" s="85" t="s">
+        <v>110</v>
+      </c>
+      <c r="D68" s="52"/>
+      <c r="E68" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="F67" s="88"/>
-      <c r="G67" s="88"/>
-      <c r="H67" s="89"/>
-    </row>
-    <row r="68" spans="1:8">
-      <c r="A68" s="93"/>
-      <c r="B68" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="C68" s="81"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F68" s="24"/>
-      <c r="G68" s="24"/>
-      <c r="H68" s="90"/>
-    </row>
-    <row r="69" spans="1:8" ht="25.5">
-      <c r="A69" s="93"/>
+      <c r="F68" s="70"/>
+      <c r="G68" s="70"/>
+      <c r="H68" s="71"/>
+    </row>
+    <row r="69" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A69" s="57">
+        <v>64</v>
+      </c>
       <c r="B69" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="C69" s="81"/>
+        <v>100</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D69" s="19"/>
       <c r="E69" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F69" s="24"/>
       <c r="G69" s="24"/>
-      <c r="H69" s="90"/>
+      <c r="H69" s="72"/>
     </row>
     <row r="70" spans="1:8" ht="25.5">
-      <c r="A70" s="93"/>
+      <c r="A70" s="53">
+        <v>65</v>
+      </c>
       <c r="B70" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C70" s="81"/>
+        <v>101</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D70" s="19"/>
       <c r="E70" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F70" s="24"/>
       <c r="G70" s="24"/>
-      <c r="H70" s="90"/>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="93"/>
+      <c r="H70" s="72"/>
+    </row>
+    <row r="71" spans="1:8" ht="26.25" thickBot="1">
+      <c r="A71" s="57">
+        <v>66</v>
+      </c>
       <c r="B71" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C71" s="81"/>
+        <v>102</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D71" s="19"/>
       <c r="E71" s="19" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F71" s="24"/>
       <c r="G71" s="24"/>
-      <c r="H71" s="90"/>
+      <c r="H71" s="72"/>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="93"/>
+      <c r="A72" s="53">
+        <v>67</v>
+      </c>
       <c r="B72" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="C72" s="81"/>
+        <v>103</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D72" s="19"/>
       <c r="E72" s="19" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="F72" s="24"/>
       <c r="G72" s="24"/>
-      <c r="H72" s="90"/>
-    </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="93"/>
+      <c r="H72" s="72"/>
+    </row>
+    <row r="73" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A73" s="57">
+        <v>68</v>
+      </c>
       <c r="B73" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="C73" s="81"/>
+        <v>104</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="D73" s="19"/>
       <c r="E73" s="19" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F73" s="24"/>
       <c r="G73" s="24"/>
-      <c r="H73" s="90"/>
-    </row>
-    <row r="74" spans="1:8" ht="13.5" thickBot="1">
-      <c r="A74" s="94"/>
-      <c r="B74" s="109" t="s">
-        <v>109</v>
-      </c>
-      <c r="C74" s="96"/>
-      <c r="D74" s="62"/>
-      <c r="E74" s="62" t="s">
+      <c r="H73" s="72"/>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="53">
+        <v>69</v>
+      </c>
+      <c r="B74" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F74" s="78"/>
-      <c r="G74" s="78"/>
-      <c r="H74" s="97"/>
-    </row>
-    <row r="75" spans="1:8">
-      <c r="A75" s="83"/>
-      <c r="B75" s="84"/>
-      <c r="C75" s="85"/>
-      <c r="D75" s="58"/>
-      <c r="E75" s="58"/>
-      <c r="F75" s="73"/>
-      <c r="G75" s="73"/>
-      <c r="H75" s="73"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="24"/>
+      <c r="H74" s="72"/>
+    </row>
+    <row r="75" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A75" s="57">
+        <v>70</v>
+      </c>
+      <c r="B75" s="83" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="D75" s="48"/>
+      <c r="E75" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="F75" s="64"/>
+      <c r="G75" s="64"/>
+      <c r="H75" s="76"/>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="80"/>
-      <c r="B76" s="21"/>
-      <c r="C76" s="81"/>
-      <c r="D76" s="19"/>
-      <c r="E76" s="19"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="24"/>
-      <c r="H76" s="24"/>
+      <c r="A76" s="66" t="s">
+        <v>112</v>
+      </c>
+      <c r="B76" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="C76" s="67" t="s">
+        <v>55</v>
+      </c>
+      <c r="D76" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" s="45"/>
+      <c r="F76" s="59">
+        <v>6</v>
+      </c>
+      <c r="G76" s="59"/>
+      <c r="H76" s="59"/>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" s="80"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="81"/>
-      <c r="D77" s="19"/>
+      <c r="A77" s="88" t="s">
+        <v>114</v>
+      </c>
+      <c r="B77" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="C77" s="89" t="s">
+        <v>55</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>6</v>
+      </c>
       <c r="E77" s="19"/>
-      <c r="F77" s="24"/>
+      <c r="F77" s="24">
+        <v>11</v>
+      </c>
       <c r="G77" s="24"/>
       <c r="H77" s="24"/>
     </row>
-    <row r="78" spans="1:8">
-      <c r="A78" s="80"/>
-      <c r="B78" s="21"/>
-      <c r="C78" s="81"/>
-      <c r="D78" s="19"/>
-      <c r="E78" s="19"/>
-      <c r="F78" s="24"/>
-      <c r="G78" s="24"/>
-      <c r="H78" s="24"/>
-    </row>
-    <row r="79" spans="1:8">
-      <c r="A79" s="80"/>
-      <c r="B79" s="21"/>
-      <c r="C79" s="81"/>
-      <c r="D79" s="19"/>
-      <c r="E79" s="19"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="24"/>
-      <c r="H79" s="24"/>
+    <row r="78" spans="1:8" s="106" customFormat="1">
+      <c r="A78" s="102"/>
+      <c r="B78" s="103"/>
+      <c r="C78" s="104"/>
+      <c r="D78" s="81"/>
+      <c r="E78" s="81"/>
+      <c r="F78" s="105"/>
+      <c r="G78" s="105"/>
+      <c r="H78" s="105"/>
+    </row>
+    <row r="79" spans="1:8" s="106" customFormat="1">
+      <c r="A79" s="102"/>
+      <c r="B79" s="103"/>
+      <c r="C79" s="104"/>
+      <c r="D79" s="81"/>
+      <c r="E79" s="81"/>
+      <c r="F79" s="105"/>
+      <c r="G79" s="105"/>
+      <c r="H79" s="105"/>
+    </row>
+    <row r="80" spans="1:8" s="106" customFormat="1">
+      <c r="A80" s="102"/>
+      <c r="B80" s="103"/>
+      <c r="C80" s="104"/>
+      <c r="D80" s="81"/>
+      <c r="E80" s="81"/>
+      <c r="F80" s="105"/>
+      <c r="G80" s="105"/>
+      <c r="H80" s="105"/>
+    </row>
+    <row r="81" spans="1:8" s="106" customFormat="1">
+      <c r="A81" s="102"/>
+      <c r="B81" s="103"/>
+      <c r="C81" s="104"/>
+      <c r="D81" s="81"/>
+      <c r="E81" s="81"/>
+      <c r="F81" s="105"/>
+      <c r="G81" s="105"/>
+      <c r="H81" s="105"/>
+    </row>
+    <row r="82" spans="1:8" s="106" customFormat="1">
+      <c r="A82" s="102"/>
+      <c r="B82" s="103"/>
+      <c r="C82" s="104"/>
+      <c r="D82" s="81"/>
+      <c r="E82" s="81"/>
+      <c r="F82" s="105"/>
+      <c r="G82" s="105"/>
+      <c r="H82" s="105"/>
     </row>
   </sheetData>
+  <autoFilter ref="F1:F80" xr:uid="{4A3DAA3C-C6B7-4DE2-BF03-29C3D6359CDF}"/>
   <mergeCells count="6">
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="C1:D2"/>
@@ -3211,7 +3575,7 @@
     <mergeCell ref="D4:E4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D39" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>FR</formula1>
     </dataValidation>
@@ -3220,7 +3584,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="79" fitToHeight="8" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="87" fitToHeight="8" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -3335,6 +3699,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>